<commit_message>
11/18/2025 ; Updated the code with addon steps
</commit_message>
<xml_diff>
--- a/src/test/resources/Test-Data-Files/TestData.xlsx
+++ b/src/test/resources/Test-Data-Files/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimma\Documents\Testing-Automation\web-ui-automation\src\test\resources\Test-Data-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2633B2-8C46-4555-9287-E8D0E1C3930C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F588BDA-A1EE-4F53-A087-091A1EFEB12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Password</t>
   </si>
@@ -91,34 +91,25 @@
     <t>Stream</t>
   </si>
   <si>
-    <t>Year of Complition</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Stream Message</t>
-  </si>
-  <si>
     <t>KG RCET</t>
   </si>
   <si>
-    <t>Electrical &amp; Electronices</t>
-  </si>
-  <si>
-    <t>B.Tech</t>
-  </si>
-  <si>
     <t>Hyderabad</t>
   </si>
   <si>
     <t>Testing the message box</t>
   </si>
   <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
-    <t>Mobile number</t>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Electrical and Electronics</t>
+  </si>
+  <si>
+    <t>Message</t>
   </si>
 </sst>
 </file>
@@ -199,7 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -221,16 +212,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -517,7 +511,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="A1:B13"/>
+      <selection activeCell="B8" sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,24 +561,24 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="9">
-        <v>990909090</v>
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>26</v>
@@ -592,59 +586,43 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2020</v>
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="12">
-        <v>35800</v>
-      </c>
+      <c r="A12" s="11"/>
+      <c r="B12" s="13"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>